<commit_message>
[IMP] Adjust SLA Purchase Report
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_sla_purchase.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_sla_purchase.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="SLA Purchase Report" sheetId="1" state="visible" r:id="rId2"/>
@@ -110,11 +110,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="#,##0_);\(#,##0\)"/>
-    <numFmt numFmtId="167" formatCode="#,##0.00_);\(#,##0.00\)"/>
+    <numFmt numFmtId="166" formatCode="#,##0"/>
+    <numFmt numFmtId="167" formatCode="#,###.00"/>
+    <numFmt numFmtId="168" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="169" formatCode="#,##0_);\(#,##0\)"/>
+    <numFmt numFmtId="170" formatCode="#,##0.00_);\(#,##0.00\)"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -200,7 +203,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -221,12 +224,20 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -237,15 +248,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -269,6 +280,14 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -277,11 +296,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -306,48 +325,44 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:12"/>
+  <dimension ref="A1:AMJ12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N5" activeCellId="0" sqref="N5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.3112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.0408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="21.2397959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.234693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="25.5561224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="22.4336734693878"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="23.280612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="28.5561224489796"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="23.3979591836735"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="4" width="19.8010204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="19.3112244897959"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="18.8367346938776"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="18.8367346938776"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="3" width="15.8367346938776"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="6" width="15.8367346938776"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="15.8367346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="5" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="23.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="23.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="23.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="23.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="23.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="2" width="23.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="23.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="5" width="23.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="6" width="23.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="3" width="23.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="7" width="23.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="8" width="23.61"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="17" style="8" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7"/>
+      <c r="A1" s="9"/>
       <c r="B1" s="0"/>
       <c r="C1" s="0"/>
       <c r="D1" s="0"/>
       <c r="E1" s="0"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="9"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="11"/>
       <c r="H1" s="0"/>
       <c r="I1" s="0"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
       <c r="M1" s="0"/>
-      <c r="N1" s="11"/>
+      <c r="N1" s="13"/>
       <c r="O1" s="0"/>
       <c r="P1" s="0"/>
       <c r="Q1" s="0"/>
@@ -1360,22 +1375,22 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="0"/>
       <c r="C2" s="0"/>
       <c r="D2" s="0"/>
       <c r="E2" s="0"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="9"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="11"/>
       <c r="H2" s="0"/>
       <c r="I2" s="0"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
       <c r="M2" s="0"/>
-      <c r="N2" s="11"/>
+      <c r="N2" s="13"/>
       <c r="O2" s="0"/>
       <c r="P2" s="0"/>
       <c r="Q2" s="0"/>
@@ -2388,24 +2403,24 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="14" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="13"/>
+      <c r="D3" s="15"/>
       <c r="E3" s="0"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="9"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
       <c r="H3" s="0"/>
       <c r="I3" s="0"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
       <c r="M3" s="0"/>
-      <c r="N3" s="11"/>
+      <c r="N3" s="13"/>
       <c r="O3" s="0"/>
       <c r="P3" s="0"/>
       <c r="Q3" s="0"/>
@@ -3418,22 +3433,22 @@
       <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="16"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="18"/>
       <c r="E4" s="0"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="9"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="11"/>
       <c r="H4" s="0"/>
       <c r="I4" s="0"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
       <c r="M4" s="0"/>
-      <c r="N4" s="11"/>
+      <c r="N4" s="13"/>
       <c r="O4" s="0"/>
       <c r="P4" s="0"/>
       <c r="Q4" s="0"/>
@@ -4446,24 +4461,24 @@
       <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="13"/>
+      <c r="D5" s="15"/>
       <c r="E5" s="0"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="9"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="11"/>
       <c r="H5" s="0"/>
       <c r="I5" s="0"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
       <c r="M5" s="0"/>
-      <c r="N5" s="11"/>
+      <c r="N5" s="13"/>
       <c r="O5" s="0"/>
       <c r="P5" s="0"/>
       <c r="Q5" s="0"/>
@@ -5476,24 +5491,24 @@
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14" t="s">
+      <c r="B6" s="19"/>
+      <c r="C6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="13"/>
+      <c r="D6" s="19"/>
       <c r="E6" s="0"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="9"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="11"/>
       <c r="H6" s="0"/>
       <c r="I6" s="0"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
       <c r="M6" s="0"/>
-      <c r="N6" s="11"/>
+      <c r="N6" s="13"/>
       <c r="O6" s="0"/>
       <c r="P6" s="0"/>
       <c r="Q6" s="0"/>
@@ -6506,22 +6521,21 @@
       <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="13"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="20"/>
       <c r="E7" s="0"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="9"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="11"/>
       <c r="H7" s="0"/>
       <c r="I7" s="0"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
       <c r="M7" s="0"/>
-      <c r="N7" s="11"/>
+      <c r="N7" s="13"/>
       <c r="O7" s="0"/>
       <c r="P7" s="0"/>
       <c r="Q7" s="0"/>
@@ -7534,22 +7548,22 @@
       <c r="AMJ7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="18"/>
       <c r="E8" s="0"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="9"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="11"/>
       <c r="H8" s="0"/>
       <c r="I8" s="0"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
       <c r="M8" s="0"/>
-      <c r="N8" s="11"/>
+      <c r="N8" s="13"/>
       <c r="O8" s="0"/>
       <c r="P8" s="0"/>
       <c r="Q8" s="0"/>
@@ -8562,22 +8576,22 @@
       <c r="AMJ8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="18"/>
       <c r="E9" s="0"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="9"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="11"/>
       <c r="H9" s="0"/>
       <c r="I9" s="0"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
       <c r="M9" s="0"/>
-      <c r="N9" s="11"/>
+      <c r="N9" s="13"/>
       <c r="O9" s="0"/>
       <c r="P9" s="0"/>
       <c r="Q9" s="0"/>
@@ -9590,22 +9604,22 @@
       <c r="AMJ9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="18"/>
       <c r="E10" s="0"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="9"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="11"/>
       <c r="H10" s="0"/>
       <c r="I10" s="0"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
       <c r="M10" s="0"/>
-      <c r="N10" s="11"/>
+      <c r="N10" s="13"/>
       <c r="O10" s="0"/>
       <c r="P10" s="0"/>
       <c r="Q10" s="0"/>
@@ -10618,20 +10632,20 @@
       <c r="AMJ10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="18"/>
       <c r="E11" s="0"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="9"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="11"/>
       <c r="H11" s="0"/>
       <c r="I11" s="0"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
       <c r="M11" s="0"/>
-      <c r="N11" s="11"/>
+      <c r="N11" s="13"/>
       <c r="O11" s="0"/>
       <c r="P11" s="0"/>
       <c r="Q11" s="0"/>
@@ -11643,60 +11657,60 @@
       <c r="AMI11" s="0"/>
       <c r="AMJ11" s="0"/>
     </row>
-    <row r="12" s="21" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="17" t="s">
+    <row r="12" s="25" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="18" t="s">
+      <c r="I12" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="20" t="s">
+      <c r="J12" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="K12" s="17" t="s">
+      <c r="K12" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="L12" s="17" t="s">
+      <c r="L12" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="M12" s="17" t="s">
+      <c r="M12" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="N12" s="19" t="s">
+      <c r="N12" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="O12" s="17" t="s">
+      <c r="O12" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="P12" s="17" t="s">
+      <c r="P12" s="21" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>